<commit_message>
Freight & Detention Bill Processing
</commit_message>
<xml_diff>
--- a/App_Templates/ErectionDocumentTemplate.xlsx
+++ b/App_Templates/ErectionDocumentTemplate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="30" windowWidth="18060" windowHeight="9090"/>
@@ -47,9 +47,6 @@
     <t>APPR</t>
   </si>
   <si>
-    <t>ERECTION DOCUMENT LIST</t>
-  </si>
-  <si>
     <t>Released or Modified Document List</t>
   </si>
   <si>
@@ -63,13 +60,16 @@
   </si>
   <si>
     <t>STATUS DATE</t>
+  </si>
+  <si>
+    <t>DOCUMENT LIST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,196 +331,39 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -528,6 +371,11 @@
       <color rgb="FFFF99CC"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -606,6 +454,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -640,6 +489,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -815,14 +665,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.5"/>
+  <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="24.7109375" style="1" customWidth="1"/>
@@ -833,39 +683,39 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:10" ht="19.5" x14ac:dyDescent="0.15">
+      <c r="A1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="20"/>
+    </row>
+    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="18"/>
-    </row>
-    <row r="2" spans="1:10" ht="12.75">
-      <c r="A2" s="20" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="15"/>
+    </row>
+    <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="22"/>
-    </row>
-    <row r="3" spans="1:10" ht="12.75">
-      <c r="A3" s="20" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="12.75">
+    </row>
+    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -878,14 +728,14 @@
       <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="24" t="s">
-        <v>15</v>
+      <c r="G4" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>7</v>
@@ -897,7 +747,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="8"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -909,7 +759,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="8"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -921,7 +771,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="9"/>
     </row>
-    <row r="7" spans="1:10" ht="11.25" thickBot="1">
+    <row r="7" spans="1:10" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -945,14 +795,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.5"/>
+  <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="24.7109375" style="1" customWidth="1"/>
@@ -963,21 +813,21 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18">
-      <c r="A1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="15"/>
-    </row>
-    <row r="2" spans="1:10" ht="12.75">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.15">
+      <c r="A1" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="8"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1021,7 +871,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="8"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1033,7 +883,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="9"/>
     </row>
-    <row r="5" spans="1:10" ht="11.25" thickBot="1">
+    <row r="5" spans="1:10" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>

</xml_diff>